<commit_message>
Rewrite pivot table test
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -6,42 +6,67 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Data" sheetId="2" r:id="rId2"/>
-    <x:sheet name="PT1" sheetId="3" r:id="rId3"/>
-    <x:sheet name="PT2" sheetId="4" r:id="rId4"/>
-    <x:sheet name="PT3" sheetId="5" r:id="rId5"/>
+    <x:sheet name="PastrySalesData" sheetId="2" r:id="rId2"/>
+    <x:sheet name="PivotTable1" sheetId="3" r:id="rId3"/>
+    <x:sheet name="PivotTable2" sheetId="4" r:id="rId4"/>
+    <x:sheet name="PivotTable3" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId8"/>
-    <x:pivotCache cacheId="1" r:id="rId11"/>
-    <x:pivotCache cacheId="2" r:id="rId14"/>
+    <x:pivotCache cacheId="0" r:id="rId9"/>
+    <x:pivotCache cacheId="1" r:id="rId12"/>
+    <x:pivotCache cacheId="2" r:id="rId15"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <x:si>
-    <x:t>Category</x:t>
+    <x:t>Name</x:t>
   </x:si>
   <x:si>
-    <x:t>Number</x:t>
+    <x:t>NumberOfOrders</x:t>
   </x:si>
   <x:si>
-    <x:t>A</x:t>
+    <x:t>Quality</x:t>
   </x:si>
   <x:si>
-    <x:t>B</x:t>
+    <x:t>Month</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Croissant</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apr</x:t>
+  </x:si>
+  <x:si>
+    <x:t>May</x:t>
+  </x:si>
+  <x:si>
+    <x:t>June</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Doughnut</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bearclaw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Danish</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Scone</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="1">
+  <x:numFmts count="2">
     <x:numFmt numFmtId="0" formatCode=""/>
+    <x:numFmt numFmtId="165" formatCode="0%"/>
   </x:numFmts>
   <x:fonts count="1">
     <x:font>
@@ -97,41 +122,80 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PT1" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="2">
-    <x:pivotField name="Category" axis="axisRow" showAll="0">
-      <x:items>
+  <x:pivotFields count="4">
+    <x:pivotField name="Name" axis="axisRow" showAll="0">
+      <x:items count="6">
         <x:item x="0"/>
         <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
         <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Number" dataField="1" showAll="0">
-      <x:items>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Quality" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Month" axis="axisCol" showAll="0">
+      <x:items count="4">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
         <x:item t="default"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
-  <x:rowFields>
+  <x:rowFields count="1">
     <x:field x="0"/>
   </x:rowFields>
-  <x:rowItems>
+  <x:rowItems count="6">
     <x:i>
       <x:x v="0"/>
     </x:i>
     <x:i>
       <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
     </x:i>
   </x:rowItems>
-  <x:colItems>
-    <x:i/>
+  <x:colFields count="1">
+    <x:field x="3"/>
+  </x:colFields>
+  <x:colItems count="4">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
   </x:colItems>
-  <x:dataFields>
-    <x:dataField name="Number" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="0" numFmtId="4294967295"/>
+  <x:dataFields count="1">
+    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -143,41 +207,82 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PT2" cacheId="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="2">
-    <x:pivotField name="Category" axis="axisRow" showAll="0">
-      <x:items>
+  <x:pivotFields count="4">
+    <x:pivotField name="Name" axis="axisRow" showAll="0">
+      <x:items count="6">
         <x:item x="0"/>
         <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
         <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Number" dataField="1" showAll="0">
-      <x:items>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Quality" dataField="1" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Month" axis="axisCol" showAll="0">
+      <x:items count="4">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
         <x:item t="default"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
-  <x:rowFields>
+  <x:rowFields count="2">
     <x:field x="0"/>
+    <x:field x="-2"/>
   </x:rowFields>
-  <x:rowItems>
+  <x:rowItems count="6">
     <x:i>
       <x:x v="0"/>
     </x:i>
     <x:i>
       <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
     </x:i>
   </x:rowItems>
-  <x:colItems>
-    <x:i/>
+  <x:colFields count="1">
+    <x:field x="3"/>
+  </x:colFields>
+  <x:colItems count="4">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
   </x:colItems>
-  <x:dataFields>
-    <x:dataField name="Number" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="0" numFmtId="4294967295"/>
+  <x:dataFields count="2">
+    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
+    <x:dataField name="Sum of Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -189,41 +294,83 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PT3" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="2">
-    <x:pivotField name="Category" axis="axisRow" showAll="0">
-      <x:items>
+  <x:pivotFields count="4">
+    <x:pivotField name="Name" axis="axisRow" showAll="0">
+      <x:items count="6">
         <x:item x="0"/>
         <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
         <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Number" dataField="1" showAll="0">
-      <x:items>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Quality" dataField="1" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Month" axis="axisCol" showAll="0">
+      <x:items count="4">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
         <x:item t="default"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
-  <x:rowFields>
+  <x:rowFields count="1">
     <x:field x="0"/>
   </x:rowFields>
-  <x:rowItems>
+  <x:rowItems count="6">
     <x:i>
       <x:x v="0"/>
     </x:i>
     <x:i>
       <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
     </x:i>
   </x:rowItems>
-  <x:colItems>
-    <x:i/>
+  <x:colFields count="2">
+    <x:field x="3"/>
+    <x:field x="-2"/>
+  </x:colFields>
+  <x:colItems count="4">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
   </x:colItems>
-  <x:dataFields>
-    <x:dataField name="Number" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="0" numFmtId="4294967295"/>
+  <x:dataFields count="3">
+    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
+    <x:dataField name="Sum of Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
+    <x:dataField name="Sum of NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -232,6 +379,19 @@
     </x:ext>
   </x:extLst>
 </x:pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PastrySalesData" displayName="PastrySalesData" ref="A1:D16" totalsRowShown="0">
+  <x:autoFilter ref="A1:D16"/>
+  <x:tableColumns count="4">
+    <x:tableColumn id="1" name="Name"/>
+    <x:tableColumn id="2" name="NumberOfOrders"/>
+    <x:tableColumn id="3" name="Quality"/>
+    <x:tableColumn id="4" name="Month"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,42 +682,240 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B4"/>
+  <x:dimension ref="A1:D16"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.720625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="16.680625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="7.970625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="7.640625" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2">
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
-        <x:v>100</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:2">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="n">
+        <x:v>60.2</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
       <x:c r="A3" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
-        <x:v>150</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:2">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>50.42</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>22.12</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="A5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="n">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="n">
+        <x:v>89.99</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="A6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="n">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="n">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="A7" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="n">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="n">
+        <x:v>75.33</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="A8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="n">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="n">
+        <x:v>10.24</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="A9" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="n">
+        <x:v>184</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="n">
+        <x:v>33.33</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="A10" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="n">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="n">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="A11" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="n">
+        <x:v>394</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="n">
+        <x:v>-20.24</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="A12" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="n">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="A13" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="n">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="n">
+        <x:v>24.76</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="A14" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="n">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="A15" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="n">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="n">
+        <x:v>5.19</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="A16" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="n">
+        <x:v>243</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="n">
+        <x:v>44.2</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -565,7 +923,9 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:tableParts count="0"/>
+  <x:tableParts count="1">
+    <x:tablePart r:id="rId11"/>
+  </x:tableParts>
 </x:worksheet>
 </file>
 
@@ -579,6 +939,9 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:1"/>
   </x:sheetData>
@@ -600,6 +963,9 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:1"/>
   </x:sheetData>
@@ -621,6 +987,9 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:1"/>
   </x:sheetData>
@@ -635,17 +1004,30 @@
 <file path=pivotCache/pivotCacheDefinition.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="'Data'!A1:B4"/>
+    <x:worksheetSource name="'PastrySalesData'!A1:D16"/>
   </x:cacheSource>
   <x:cacheFields>
-    <x:cacheField name="Category">
+    <x:cacheField name="Name">
       <x:sharedItems>
-        <x:s v="A"/>
-        <x:s v="B"/>
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
       </x:sharedItems>
     </x:cacheField>
-    <x:cacheField name="Number">
+    <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems>
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="June"/>
+      </x:sharedItems>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -654,17 +1036,30 @@
 <file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="'Data'!A1:B4"/>
+    <x:worksheetSource name="'PastrySalesData'!A1:D16"/>
   </x:cacheSource>
   <x:cacheFields>
-    <x:cacheField name="Category">
+    <x:cacheField name="Name">
       <x:sharedItems>
-        <x:s v="A"/>
-        <x:s v="B"/>
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
       </x:sharedItems>
     </x:cacheField>
-    <x:cacheField name="Number">
+    <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems>
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="June"/>
+      </x:sharedItems>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -673,17 +1068,30 @@
 <file path=pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="'Data'!A1:B4"/>
+    <x:worksheetSource name="'PastrySalesData'!A1:D16"/>
   </x:cacheSource>
   <x:cacheFields>
-    <x:cacheField name="Category">
+    <x:cacheField name="Name">
       <x:sharedItems>
-        <x:s v="A"/>
-        <x:s v="B"/>
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
       </x:sharedItems>
     </x:cacheField>
-    <x:cacheField name="Number">
+    <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems>
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="June"/>
+      </x:sharedItems>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>

</xml_diff>

<commit_message>
More pivot table fixes - for when there are no column labels
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -10,13 +10,15 @@
     <x:sheet name="PivotTable1" sheetId="3" r:id="rId3"/>
     <x:sheet name="PivotTable2" sheetId="4" r:id="rId4"/>
     <x:sheet name="PivotTable3" sheetId="5" r:id="rId5"/>
+    <x:sheet name="PivotTableNoColumnLabels" sheetId="6" r:id="rId6"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId9"/>
-    <x:pivotCache cacheId="1" r:id="rId12"/>
-    <x:pivotCache cacheId="2" r:id="rId15"/>
+    <x:pivotCache cacheId="0" r:id="rId10"/>
+    <x:pivotCache cacheId="1" r:id="rId13"/>
+    <x:pivotCache cacheId="2" r:id="rId16"/>
+    <x:pivotCache cacheId="3" r:id="rId19"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
@@ -371,6 +373,99 @@
     <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
     <x:dataField name="Sum of Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
     <x:dataField name="Sum of NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+  </x:dataFields>
+  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
+    </x:ext>
+  </x:extLst>
+</x:pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTableNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:pivotFields count="4">
+    <x:pivotField name="Name" axis="axisRow" showAll="0">
+      <x:items count="6">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Quality" dataField="1" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Month" axis="axisRow" showAll="0">
+      <x:items count="4">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+  </x:pivotFields>
+  <x:rowFields count="2">
+    <x:field x="0"/>
+    <x:field x="3"/>
+  </x:rowFields>
+  <x:rowItems count="10">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:rowItems>
+  <x:colFields count="1">
+    <x:field x="-2"/>
+  </x:colFields>
+  <x:colItems count="2">
+    <x:i i="0">
+      <x:x v="0"/>
+    </x:i>
+    <x:i i="1">
+      <x:x v="1"/>
+    </x:i>
+  </x:colItems>
+  <x:dataFields count="2">
+    <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -924,7 +1019,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId11"/>
+    <x:tablePart r:id="rId14"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1001,6 +1096,27 @@
 </x:worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
 <file path=pivotCache/pivotCacheDefinition.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
@@ -1097,6 +1213,38 @@
 </x:pivotCacheDefinition>
 </file>
 
+<file path=pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="'PastrySalesData'!A1:D16"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems>
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems>
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="June"/>
+      </x:sharedItems>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
 <file path=pivotCache/pivotCacheRecords.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1107,4 +1255,8 @@
 
 <file path=pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>

<commit_message>
Use case-insensitive lookup for generating cacheFields element.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -60,6 +60,12 @@
   </x:si>
   <x:si>
     <x:t>Scone</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SconE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SCONE</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -987,7 +993,7 @@
     </x:row>
     <x:row r="15" spans="1:4">
       <x:c r="A15" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B15" s="0" t="n">
         <x:v>122</x:v>
@@ -1001,7 +1007,7 @@
     </x:row>
     <x:row r="16" spans="1:4">
       <x:c r="A16" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B16" s="0" t="n">
         <x:v>243</x:v>

</xml_diff>

<commit_message>
Add pivot table to test for when field is both a label and a value field.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -7,18 +7,20 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="PastrySalesData" sheetId="2" r:id="rId2"/>
-    <x:sheet name="PivotTable1" sheetId="3" r:id="rId3"/>
-    <x:sheet name="PivotTable2" sheetId="4" r:id="rId4"/>
-    <x:sheet name="PivotTable3" sheetId="5" r:id="rId5"/>
-    <x:sheet name="PivotTableNoColumnLabels" sheetId="6" r:id="rId6"/>
+    <x:sheet name="pvt1" sheetId="3" r:id="rId3"/>
+    <x:sheet name="pvt2" sheetId="4" r:id="rId4"/>
+    <x:sheet name="pvt3" sheetId="5" r:id="rId5"/>
+    <x:sheet name="pvtNoColumnLabels" sheetId="6" r:id="rId6"/>
+    <x:sheet name="pvtFieldAsValueAndLabel" sheetId="7" r:id="rId7"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId10"/>
-    <x:pivotCache cacheId="1" r:id="rId13"/>
-    <x:pivotCache cacheId="2" r:id="rId16"/>
-    <x:pivotCache cacheId="3" r:id="rId19"/>
+    <x:pivotCache cacheId="0" r:id="rId11"/>
+    <x:pivotCache cacheId="1" r:id="rId14"/>
+    <x:pivotCache cacheId="2" r:id="rId17"/>
+    <x:pivotCache cacheId="3" r:id="rId20"/>
+    <x:pivotCache cacheId="4" r:id="rId23"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
@@ -130,7 +132,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0">
@@ -215,7 +217,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0">
@@ -302,7 +304,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0">
@@ -390,7 +392,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTableNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0">
@@ -472,6 +474,92 @@
   <x:dataFields count="2">
     <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
     <x:dataField name="Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+  </x:dataFields>
+  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
+    </x:ext>
+  </x:extLst>
+</x:pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:pivotFields count="4">
+    <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0">
+      <x:items count="6">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="NumberOfOrders" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Quality" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Month" axis="axisRow" showAll="0">
+      <x:items count="4">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+  </x:pivotFields>
+  <x:rowFields count="2">
+    <x:field x="0"/>
+    <x:field x="3"/>
+  </x:rowFields>
+  <x:rowItems count="10">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:rowItems>
+  <x:colItems count="1">
+    <x:i i="0">
+      <x:x v="0"/>
+    </x:i>
+  </x:colItems>
+  <x:dataFields count="1">
+    <x:dataField name="Name" fld="0" subtotal="count" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -1025,7 +1113,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId14"/>
+    <x:tablePart r:id="rId15"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1123,6 +1211,27 @@
 </x:worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
 <file path=pivotCache/pivotCacheDefinition.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
@@ -1251,6 +1360,38 @@
 </x:pivotCacheDefinition>
 </file>
 
+<file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="'PastrySalesData'!A1:D16"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems>
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems>
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="June"/>
+      </x:sharedItems>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
 <file path=pivotCache/pivotCacheRecords.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1265,4 +1406,8 @@
 
 <file path=pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>

<commit_message>
Add unit test for collapsed pivot table fields
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -11,16 +11,18 @@
     <x:sheet name="pvt2" sheetId="4" r:id="rId4"/>
     <x:sheet name="pvt3" sheetId="5" r:id="rId5"/>
     <x:sheet name="pvtNoColumnLabels" sheetId="6" r:id="rId6"/>
-    <x:sheet name="pvtFieldAsValueAndLabel" sheetId="7" r:id="rId7"/>
+    <x:sheet name="pvtCollapsedFields" sheetId="7" r:id="rId7"/>
+    <x:sheet name="pvtFieldAsValueAndLabel" sheetId="8" r:id="rId8"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId11"/>
-    <x:pivotCache cacheId="1" r:id="rId14"/>
-    <x:pivotCache cacheId="2" r:id="rId17"/>
-    <x:pivotCache cacheId="3" r:id="rId20"/>
-    <x:pivotCache cacheId="4" r:id="rId23"/>
+    <x:pivotCache cacheId="0" r:id="rId12"/>
+    <x:pivotCache cacheId="1" r:id="rId15"/>
+    <x:pivotCache cacheId="2" r:id="rId18"/>
+    <x:pivotCache cacheId="3" r:id="rId21"/>
+    <x:pivotCache cacheId="4" r:id="rId24"/>
+    <x:pivotCache cacheId="5" r:id="rId27"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
@@ -485,7 +487,100 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:pivotFields count="4">
+    <x:pivotField name="Name" axis="axisRow" showAll="0">
+      <x:items count="6">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Quality" dataField="1" showAll="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Month" axis="axisRow" showAll="0">
+      <x:items count="4">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+  </x:pivotFields>
+  <x:rowFields count="2">
+    <x:field x="0"/>
+    <x:field x="3"/>
+  </x:rowFields>
+  <x:rowItems count="10">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:rowItems>
+  <x:colFields count="1">
+    <x:field x="-2"/>
+  </x:colFields>
+  <x:colItems count="2">
+    <x:i i="0">
+      <x:x v="0"/>
+    </x:i>
+    <x:i i="1">
+      <x:x v="1"/>
+    </x:i>
+  </x:colItems>
+  <x:dataFields count="2">
+    <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+  </x:dataFields>
+  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
+    </x:ext>
+  </x:extLst>
+</x:pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0">
@@ -1113,7 +1208,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId15"/>
+    <x:tablePart r:id="rId17"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1232,6 +1327,27 @@
 </x:worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
 <file path=pivotCache/pivotCacheDefinition.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
@@ -1392,6 +1508,38 @@
 </x:pivotCacheDefinition>
 </file>
 
+<file path=pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="'PastrySalesData'!A1:D16"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems>
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems>
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="June"/>
+      </x:sharedItems>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
 <file path=pivotCache/pivotCacheRecords.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1410,4 +1558,8 @@
 
 <file path=pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>

<commit_message>
Update pivot table reference file.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0">
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0">
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0">
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTableNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" gridDropZones="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTableNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0">

</xml_diff>

<commit_message>
Resolve conflicts after rebase.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -492,11 +492,11 @@
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0">
       <x:items count="6">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
+        <x:item sd="0" x="0"/>
+        <x:item sd="0" x="1"/>
+        <x:item sd="0" x="2"/>
+        <x:item sd="0" x="3"/>
+        <x:item sd="0" x="4"/>
         <x:item t="default"/>
       </x:items>
     </x:pivotField>
@@ -512,9 +512,9 @@
     </x:pivotField>
     <x:pivotField name="Month" axis="axisRow" showAll="0">
       <x:items count="4">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
+        <x:item sd="0" x="0"/>
+        <x:item sd="0" x="1"/>
+        <x:item sd="0" x="2"/>
         <x:item t="default"/>
       </x:items>
     </x:pivotField>

</xml_diff>

<commit_message>
Fix pivot table subtotals.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -13,16 +13,18 @@
     <x:sheet name="pvtNoColumnLabels" sheetId="6" r:id="rId6"/>
     <x:sheet name="pvtCollapsedFields" sheetId="7" r:id="rId7"/>
     <x:sheet name="pvtFieldAsValueAndLabel" sheetId="8" r:id="rId8"/>
+    <x:sheet name="pvtHideSubTotals" sheetId="9" r:id="rId9"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId12"/>
-    <x:pivotCache cacheId="1" r:id="rId15"/>
-    <x:pivotCache cacheId="2" r:id="rId18"/>
-    <x:pivotCache cacheId="3" r:id="rId21"/>
-    <x:pivotCache cacheId="4" r:id="rId24"/>
-    <x:pivotCache cacheId="5" r:id="rId27"/>
+    <x:pivotCache cacheId="0" r:id="rId13"/>
+    <x:pivotCache cacheId="1" r:id="rId16"/>
+    <x:pivotCache cacheId="2" r:id="rId19"/>
+    <x:pivotCache cacheId="3" r:id="rId22"/>
+    <x:pivotCache cacheId="4" r:id="rId25"/>
+    <x:pivotCache cacheId="5" r:id="rId28"/>
+    <x:pivotCache cacheId="6" r:id="rId31"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
@@ -137,32 +139,22 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
-    <x:pivotField name="Name" axis="axisRow" showAll="0">
-      <x:items count="6">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
         <x:item x="3"/>
         <x:item x="4"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Quality" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Month" axis="axisCol" showAll="0">
-      <x:items count="4">
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
@@ -222,32 +214,22 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
-    <x:pivotField name="Name" axis="axisRow" showAll="0">
-      <x:items count="6">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
         <x:item x="3"/>
         <x:item x="4"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Quality" dataField="1" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Month" axis="axisCol" showAll="0">
-      <x:items count="4">
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
@@ -309,32 +291,22 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
-    <x:pivotField name="Name" axis="axisRow" showAll="0">
-      <x:items count="6">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
         <x:item x="3"/>
         <x:item x="4"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Quality" dataField="1" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Month" axis="axisCol" showAll="0">
-      <x:items count="4">
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
@@ -397,32 +369,22 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
-    <x:pivotField name="Name" axis="axisRow" showAll="0">
-      <x:items count="6">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
         <x:item x="3"/>
         <x:item x="4"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Quality" dataField="1" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Month" axis="axisRow" showAll="0">
-      <x:items count="4">
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
@@ -490,32 +452,22 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
-    <x:pivotField name="Name" axis="axisRow" showAll="0">
-      <x:items count="6">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
         <x:item sd="0" x="0"/>
         <x:item sd="0" x="1"/>
         <x:item sd="0" x="2"/>
         <x:item sd="0" x="3"/>
         <x:item sd="0" x="4"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Quality" dataField="1" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Month" axis="axisRow" showAll="0">
-      <x:items count="4">
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
         <x:item sd="0" x="0"/>
         <x:item sd="0" x="1"/>
         <x:item sd="0" x="2"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
@@ -583,32 +535,22 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
-    <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0">
-      <x:items count="6">
+    <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
         <x:item x="3"/>
         <x:item x="4"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="NumberOfOrders" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Quality" showAll="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Month" axis="axisRow" showAll="0">
-      <x:items count="4">
+    <x:pivotField name="NumberOfOrders" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
-        <x:item t="default"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
@@ -655,6 +597,81 @@
   </x:colItems>
   <x:dataFields count="1">
     <x:dataField name="Name" fld="0" subtotal="count" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+  </x:dataFields>
+  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
+    </x:ext>
+  </x:extLst>
+</x:pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:pivotFields count="4">
+    <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+      </x:items>
+    </x:pivotField>
+  </x:pivotFields>
+  <x:rowFields count="1">
+    <x:field x="-2"/>
+  </x:rowFields>
+  <x:colFields count="2">
+    <x:field x="0"/>
+    <x:field x="3"/>
+  </x:colFields>
+  <x:colItems count="10">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:colItems>
+  <x:dataFields count="2">
+    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
+    <x:dataField name="Sum of Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -1208,7 +1225,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId17"/>
+    <x:tablePart r:id="rId20"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1348,6 +1365,30 @@
 </x:worksheet>
 </file>
 
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:1"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
 <file path=pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
@@ -1540,6 +1581,38 @@
 </x:pivotCacheDefinition>
 </file>
 
+<file path=pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems>
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems>
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="June"/>
+      </x:sharedItems>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
 <file path=pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1562,4 +1635,8 @@
 
 <file path=pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>

<commit_message>
Update pivot table examples
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -14,23 +14,25 @@
     <x:sheet name="pvtCollapsedFields" sheetId="7" r:id="rId7"/>
     <x:sheet name="pvtFieldAsValueAndLabel" sheetId="8" r:id="rId8"/>
     <x:sheet name="pvtHideSubTotals" sheetId="9" r:id="rId9"/>
+    <x:sheet name="pvtFilter" sheetId="10" r:id="rId10"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId13"/>
-    <x:pivotCache cacheId="1" r:id="rId16"/>
-    <x:pivotCache cacheId="2" r:id="rId19"/>
-    <x:pivotCache cacheId="3" r:id="rId22"/>
-    <x:pivotCache cacheId="4" r:id="rId25"/>
-    <x:pivotCache cacheId="5" r:id="rId28"/>
-    <x:pivotCache cacheId="6" r:id="rId31"/>
+    <x:pivotCache cacheId="0" r:id="rId14"/>
+    <x:pivotCache cacheId="1" r:id="rId17"/>
+    <x:pivotCache cacheId="2" r:id="rId20"/>
+    <x:pivotCache cacheId="3" r:id="rId23"/>
+    <x:pivotCache cacheId="4" r:id="rId26"/>
+    <x:pivotCache cacheId="5" r:id="rId29"/>
+    <x:pivotCache cacheId="6" r:id="rId32"/>
+    <x:pivotCache cacheId="7" r:id="rId35"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -44,6 +46,9 @@
     <x:t>Month</x:t>
   </x:si>
   <x:si>
+    <x:t>BakeDate</x:t>
+  </x:si>
+  <x:si>
     <x:t>Croissant</x:t>
   </x:si>
   <x:si>
@@ -53,7 +58,7 @@
     <x:t>May</x:t>
   </x:si>
   <x:si>
-    <x:t>June</x:t>
+    <x:t>Jun</x:t>
   </x:si>
   <x:si>
     <x:t>Doughnut</x:t>
@@ -118,13 +123,20 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -138,7 +150,7 @@
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -157,6 +169,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="0"/>
@@ -213,7 +226,7 @@
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -232,6 +245,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -290,7 +304,7 @@
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -309,6 +323,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="0"/>
@@ -366,9 +381,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" rowHeaderCaption="Pastry name" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -387,6 +402,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -451,7 +467,7 @@
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item sd="0" x="0"/>
@@ -470,6 +486,7 @@
         <x:item sd="0" x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -534,7 +551,7 @@
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -553,6 +570,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -608,9 +626,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" colHeaderCaption="Measures" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -629,6 +647,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="-2"/>
@@ -682,14 +701,114 @@
 </x:pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+  <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <x:pivotFields count="5">
+    <x:pivotField name="Name" axis="axisPage" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" axis="axisPage" showAll="0" defaultSubtotal="0">
+      <x:items count="15">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+        <x:item x="5"/>
+        <x:item x="6"/>
+        <x:item x="7"/>
+        <x:item x="8"/>
+        <x:item x="9"/>
+        <x:item x="10"/>
+        <x:item x="11"/>
+        <x:item x="12"/>
+        <x:item x="13"/>
+        <x:item x="14"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="BakeDate" axis="axisPage" showAll="0" defaultSubtotal="0">
+      <x:items count="15">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+        <x:item x="5"/>
+        <x:item x="6"/>
+        <x:item x="7"/>
+        <x:item x="8"/>
+        <x:item x="9"/>
+        <x:item x="10"/>
+        <x:item x="11"/>
+        <x:item x="12"/>
+        <x:item x="13"/>
+        <x:item x="14"/>
+      </x:items>
+    </x:pivotField>
+  </x:pivotFields>
+  <x:rowFields count="1">
+    <x:field x="3"/>
+  </x:rowFields>
+  <x:rowItems count="4">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:rowItems>
+  <x:colItems count="1">
+    <x:i i="0">
+      <x:x v="0"/>
+    </x:i>
+  </x:colItems>
+  <x:pageFields count="3">
+    <x:pageField fld="0" item="4" hier="-1"/>
+    <x:pageField fld="2" item="13" hier="-1"/>
+    <x:pageField fld="4" item="13" hier="-1"/>
+  </x:pageFields>
+  <x:dataFields count="1">
+    <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+  </x:dataFields>
+  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
+    </x:ext>
+  </x:extLst>
+</x:pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PastrySalesData" displayName="PastrySalesData" ref="A1:D16" totalsRowShown="0">
-  <x:autoFilter ref="A1:D16"/>
-  <x:tableColumns count="4">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PastrySalesData" displayName="PastrySalesData" ref="A1:E16" totalsRowShown="0">
+  <x:autoFilter ref="A1:E16"/>
+  <x:tableColumns count="5">
     <x:tableColumn id="1" name="Name"/>
     <x:tableColumn id="2" name="NumberOfOrders"/>
     <x:tableColumn id="3" name="Quality"/>
     <x:tableColumn id="4" name="Month"/>
+    <x:tableColumn id="5" name="BakeDate"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -983,7 +1102,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D16"/>
+  <x:dimension ref="A1:E16"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -993,9 +1112,10 @@
     <x:col min="2" max="2" width="19.395425" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="10.685425" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="10.355425" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="12.735425" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -1008,10 +1128,13 @@
       <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
+    <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
         <x:v>150</x:v>
@@ -1020,12 +1143,15 @@
         <x:v>60.2</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E2" s="1">
+        <x:v>42481</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5">
+      <x:c r="A3" s="0" t="s">
         <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s">
-        <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
         <x:v>250</x:v>
@@ -1034,12 +1160,15 @@
         <x:v>50.42</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E3" s="1">
+        <x:v>42493</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
         <x:v>134</x:v>
@@ -1048,12 +1177,15 @@
         <x:v>22.12</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E4" s="1">
+        <x:v>42545</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4">
+    <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B5" s="0" t="n">
         <x:v>250</x:v>
@@ -1062,12 +1194,15 @@
         <x:v>89.99</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E5" s="1">
+        <x:v>42848</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4">
+    <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B6" s="0" t="n">
         <x:v>225</x:v>
@@ -1076,12 +1211,15 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E6" s="1">
+        <x:v>42514</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:4">
+    <x:row r="7" spans="1:5">
       <x:c r="A7" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B7" s="0" t="n">
         <x:v>210</x:v>
@@ -1090,12 +1228,15 @@
         <x:v>75.33</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E7" s="1">
+        <x:v>42523</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:4">
+    <x:row r="8" spans="1:5">
       <x:c r="A8" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B8" s="0" t="n">
         <x:v>134</x:v>
@@ -1104,12 +1245,15 @@
         <x:v>10.24</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E8" s="1">
+        <x:v>42487</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:4">
+    <x:row r="9" spans="1:5">
       <x:c r="A9" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B9" s="0" t="n">
         <x:v>184</x:v>
@@ -1118,12 +1262,15 @@
         <x:v>33.33</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E9" s="1">
+        <x:v>42510</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:4">
+    <x:row r="10" spans="1:5">
       <x:c r="A10" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B10" s="0" t="n">
         <x:v>124</x:v>
@@ -1132,12 +1279,15 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E10" s="1">
+        <x:v>42891</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:4">
+    <x:row r="11" spans="1:5">
       <x:c r="A11" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B11" s="0" t="n">
         <x:v>394</x:v>
@@ -1146,12 +1296,15 @@
         <x:v>-20.24</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E11" s="1">
+        <x:v>42849</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:4">
+    <x:row r="12" spans="1:5">
       <x:c r="A12" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="0" t="n">
         <x:v>190</x:v>
@@ -1160,12 +1313,15 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E12" s="1">
+        <x:v>42863</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:4">
+    <x:row r="13" spans="1:5">
       <x:c r="A13" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B13" s="0" t="n">
         <x:v>221</x:v>
@@ -1174,12 +1330,15 @@
         <x:v>24.76</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E13" s="1">
+        <x:v>42542</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:4">
+    <x:row r="14" spans="1:5">
       <x:c r="A14" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B14" s="0" t="n">
         <x:v>135</x:v>
@@ -1188,12 +1347,15 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E14" s="1">
+        <x:v>42847</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:4">
+    <x:row r="15" spans="1:5">
       <x:c r="A15" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B15" s="0" t="n">
         <x:v>122</x:v>
@@ -1202,12 +1364,15 @@
         <x:v>5.19</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E15" s="1">
+        <x:v>42858</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:4">
+    <x:row r="16" spans="1:5">
       <x:c r="A16" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B16" s="0" t="n">
         <x:v>243</x:v>
@@ -1216,7 +1381,10 @@
         <x:v>44.2</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E16" s="1">
+        <x:v>42900</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1225,7 +1393,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId20"/>
+    <x:tablePart r:id="rId21"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1375,14 +1543,33 @@
 </x:worksheet>
 </file>
 
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
 <file path=pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1391,17 +1578,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1410,11 +1600,11 @@
 <file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1423,17 +1613,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1442,11 +1635,11 @@
 <file path=pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1455,17 +1648,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1474,11 +1670,11 @@
 <file path=pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1487,17 +1683,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1506,11 +1705,11 @@
 <file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1519,17 +1718,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1538,11 +1740,11 @@
 <file path=pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1551,17 +1753,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1570,11 +1775,11 @@
 <file path=pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1583,22 +1788,92 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
 </file>
 
+<file path=pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15">
+        <x:n v="60.2"/>
+        <x:n v="50.42"/>
+        <x:n v="22.12"/>
+        <x:n v="89.99"/>
+        <x:n v="70"/>
+        <x:n v="75.33"/>
+        <x:n v="10.24"/>
+        <x:n v="33.33"/>
+        <x:n v="25"/>
+        <x:n v="-20.24"/>
+        <x:n v="60"/>
+        <x:n v="24.76"/>
+        <x:n v="0"/>
+        <x:n v="5.19"/>
+        <x:n v="44.2"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
+        <x:d v="2016-04-21T00:00:00"/>
+        <x:d v="2016-05-03T00:00:00"/>
+        <x:d v="2016-06-24T00:00:00"/>
+        <x:d v="2017-04-23T00:00:00"/>
+        <x:d v="2016-05-24T00:00:00"/>
+        <x:d v="2016-06-02T00:00:00"/>
+        <x:d v="2016-04-27T00:00:00"/>
+        <x:d v="2016-05-20T00:00:00"/>
+        <x:d v="2017-06-05T00:00:00"/>
+        <x:d v="2017-04-24T00:00:00"/>
+        <x:d v="2017-05-08T00:00:00"/>
+        <x:d v="2016-06-21T00:00:00"/>
+        <x:d v="2017-04-22T00:00:00"/>
+        <x:d v="2017-05-03T00:00:00"/>
+        <x:d v="2017-06-14T00:00:00"/>
+      </x:sharedItems>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
 <file path=pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1625,4 +1900,8 @@
 
 <file path=pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=pivotCache/pivotCacheRecords8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>

<commit_message>
Implement filters with multiple selected values
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -705,12 +705,12 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="5">
-    <x:pivotField name="Name" axis="axisPage" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
-        <x:item x="0"/>
+        <x:item h="1" x="0"/>
         <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
+        <x:item h="1" x="2"/>
+        <x:item h="1" x="3"/>
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
@@ -784,7 +784,7 @@
     </x:i>
   </x:colItems>
   <x:pageFields count="3">
-    <x:pageField fld="0" item="4" hier="-1"/>
+    <x:pageField fld="0" hier="-1"/>
     <x:pageField fld="2" item="13" hier="-1"/>
     <x:pageField fld="4" item="13" hier="-1"/>
   </x:pageFields>

</xml_diff>

<commit_message>
Implement pivot table row and column header captions
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -366,7 +366,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" rowHeaderCaption="Pastry name" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -608,7 +608,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" colHeaderCaption="Measures" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="4">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">

</xml_diff>

<commit_message>
Update reference pivot table file
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" rowHeaderCaption="Pastry name" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -626,7 +626,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" colHeaderCaption="Measures" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">

</xml_diff>

<commit_message>
Pivot table default filter (#508)
* Make pivot table shared strings internal only

* Clean up TestHelper

* Save selected values in filters

* Implement DateTime type in saving pivot tables

* Implement loading of pivot table filters

* Update pivot table examples

* Implement filters with multiple selected values

* Update reference pivot table file
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -14,23 +14,25 @@
     <x:sheet name="pvtCollapsedFields" sheetId="7" r:id="rId7"/>
     <x:sheet name="pvtFieldAsValueAndLabel" sheetId="8" r:id="rId8"/>
     <x:sheet name="pvtHideSubTotals" sheetId="9" r:id="rId9"/>
+    <x:sheet name="pvtFilter" sheetId="10" r:id="rId10"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId13"/>
-    <x:pivotCache cacheId="1" r:id="rId16"/>
-    <x:pivotCache cacheId="2" r:id="rId19"/>
-    <x:pivotCache cacheId="3" r:id="rId22"/>
-    <x:pivotCache cacheId="4" r:id="rId25"/>
-    <x:pivotCache cacheId="5" r:id="rId28"/>
-    <x:pivotCache cacheId="6" r:id="rId31"/>
+    <x:pivotCache cacheId="0" r:id="rId14"/>
+    <x:pivotCache cacheId="1" r:id="rId17"/>
+    <x:pivotCache cacheId="2" r:id="rId20"/>
+    <x:pivotCache cacheId="3" r:id="rId23"/>
+    <x:pivotCache cacheId="4" r:id="rId26"/>
+    <x:pivotCache cacheId="5" r:id="rId29"/>
+    <x:pivotCache cacheId="6" r:id="rId32"/>
+    <x:pivotCache cacheId="7" r:id="rId35"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -44,6 +46,9 @@
     <x:t>Month</x:t>
   </x:si>
   <x:si>
+    <x:t>BakeDate</x:t>
+  </x:si>
+  <x:si>
     <x:t>Croissant</x:t>
   </x:si>
   <x:si>
@@ -53,7 +58,7 @@
     <x:t>May</x:t>
   </x:si>
   <x:si>
-    <x:t>June</x:t>
+    <x:t>Jun</x:t>
   </x:si>
   <x:si>
     <x:t>Doughnut</x:t>
@@ -118,13 +123,20 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -138,7 +150,7 @@
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -157,6 +169,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="0"/>
@@ -213,7 +226,7 @@
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -232,6 +245,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -290,7 +304,7 @@
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -309,6 +323,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="0"/>
@@ -368,7 +383,7 @@
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" rowHeaderCaption="Pastry name" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -387,6 +402,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -451,7 +467,7 @@
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item sd="0" x="0"/>
@@ -470,6 +486,7 @@
         <x:item sd="0" x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -534,7 +551,7 @@
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -553,6 +570,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -610,7 +628,7 @@
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" colHeaderCaption="Measures" fieldListSortAscending="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="4">
+  <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -629,6 +647,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="-2"/>
@@ -682,14 +701,114 @@
 </x:pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+  <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <x:pivotFields count="5">
+    <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
+        <x:item h="1" x="0"/>
+        <x:item x="1"/>
+        <x:item h="1" x="2"/>
+        <x:item h="1" x="3"/>
+        <x:item x="4"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" axis="axisPage" showAll="0" defaultSubtotal="0">
+      <x:items count="15">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+        <x:item x="5"/>
+        <x:item x="6"/>
+        <x:item x="7"/>
+        <x:item x="8"/>
+        <x:item x="9"/>
+        <x:item x="10"/>
+        <x:item x="11"/>
+        <x:item x="12"/>
+        <x:item x="13"/>
+        <x:item x="14"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="BakeDate" axis="axisPage" showAll="0" defaultSubtotal="0">
+      <x:items count="15">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+        <x:item x="5"/>
+        <x:item x="6"/>
+        <x:item x="7"/>
+        <x:item x="8"/>
+        <x:item x="9"/>
+        <x:item x="10"/>
+        <x:item x="11"/>
+        <x:item x="12"/>
+        <x:item x="13"/>
+        <x:item x="14"/>
+      </x:items>
+    </x:pivotField>
+  </x:pivotFields>
+  <x:rowFields count="1">
+    <x:field x="3"/>
+  </x:rowFields>
+  <x:rowItems count="4">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:rowItems>
+  <x:colItems count="1">
+    <x:i i="0">
+      <x:x v="0"/>
+    </x:i>
+  </x:colItems>
+  <x:pageFields count="3">
+    <x:pageField fld="0" hier="-1"/>
+    <x:pageField fld="2" item="13" hier="-1"/>
+    <x:pageField fld="4" item="13" hier="-1"/>
+  </x:pageFields>
+  <x:dataFields count="1">
+    <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+  </x:dataFields>
+  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
+    </x:ext>
+  </x:extLst>
+</x:pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PastrySalesData" displayName="PastrySalesData" ref="A1:D16" totalsRowShown="0">
-  <x:autoFilter ref="A1:D16"/>
-  <x:tableColumns count="4">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PastrySalesData" displayName="PastrySalesData" ref="A1:E16" totalsRowShown="0">
+  <x:autoFilter ref="A1:E16"/>
+  <x:tableColumns count="5">
     <x:tableColumn id="1" name="Name"/>
     <x:tableColumn id="2" name="NumberOfOrders"/>
     <x:tableColumn id="3" name="Quality"/>
     <x:tableColumn id="4" name="Month"/>
+    <x:tableColumn id="5" name="BakeDate"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -983,7 +1102,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D16"/>
+  <x:dimension ref="A1:E16"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -993,9 +1112,10 @@
     <x:col min="2" max="2" width="19.395425" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="10.685425" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="10.355425" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="12.735425" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -1008,10 +1128,13 @@
       <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
+    <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
         <x:v>150</x:v>
@@ -1020,12 +1143,15 @@
         <x:v>60.2</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E2" s="1">
+        <x:v>42481</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5">
+      <x:c r="A3" s="0" t="s">
         <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="A3" s="0" t="s">
-        <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
         <x:v>250</x:v>
@@ -1034,12 +1160,15 @@
         <x:v>50.42</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E3" s="1">
+        <x:v>42493</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
         <x:v>134</x:v>
@@ -1048,12 +1177,15 @@
         <x:v>22.12</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E4" s="1">
+        <x:v>42545</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4">
+    <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B5" s="0" t="n">
         <x:v>250</x:v>
@@ -1062,12 +1194,15 @@
         <x:v>89.99</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E5" s="1">
+        <x:v>42848</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4">
+    <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B6" s="0" t="n">
         <x:v>225</x:v>
@@ -1076,12 +1211,15 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E6" s="1">
+        <x:v>42514</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:4">
+    <x:row r="7" spans="1:5">
       <x:c r="A7" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B7" s="0" t="n">
         <x:v>210</x:v>
@@ -1090,12 +1228,15 @@
         <x:v>75.33</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E7" s="1">
+        <x:v>42523</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:4">
+    <x:row r="8" spans="1:5">
       <x:c r="A8" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B8" s="0" t="n">
         <x:v>134</x:v>
@@ -1104,12 +1245,15 @@
         <x:v>10.24</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E8" s="1">
+        <x:v>42487</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:4">
+    <x:row r="9" spans="1:5">
       <x:c r="A9" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B9" s="0" t="n">
         <x:v>184</x:v>
@@ -1118,12 +1262,15 @@
         <x:v>33.33</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E9" s="1">
+        <x:v>42510</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:4">
+    <x:row r="10" spans="1:5">
       <x:c r="A10" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B10" s="0" t="n">
         <x:v>124</x:v>
@@ -1132,12 +1279,15 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E10" s="1">
+        <x:v>42891</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:4">
+    <x:row r="11" spans="1:5">
       <x:c r="A11" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B11" s="0" t="n">
         <x:v>394</x:v>
@@ -1146,12 +1296,15 @@
         <x:v>-20.24</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E11" s="1">
+        <x:v>42849</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:4">
+    <x:row r="12" spans="1:5">
       <x:c r="A12" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="0" t="n">
         <x:v>190</x:v>
@@ -1160,12 +1313,15 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E12" s="1">
+        <x:v>42863</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:4">
+    <x:row r="13" spans="1:5">
       <x:c r="A13" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B13" s="0" t="n">
         <x:v>221</x:v>
@@ -1174,12 +1330,15 @@
         <x:v>24.76</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E13" s="1">
+        <x:v>42542</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:4">
+    <x:row r="14" spans="1:5">
       <x:c r="A14" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B14" s="0" t="n">
         <x:v>135</x:v>
@@ -1188,12 +1347,15 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E14" s="1">
+        <x:v>42847</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:4">
+    <x:row r="15" spans="1:5">
       <x:c r="A15" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B15" s="0" t="n">
         <x:v>122</x:v>
@@ -1202,12 +1364,15 @@
         <x:v>5.19</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E15" s="1">
+        <x:v>42858</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:4">
+    <x:row r="16" spans="1:5">
       <x:c r="A16" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B16" s="0" t="n">
         <x:v>243</x:v>
@@ -1216,7 +1381,10 @@
         <x:v>44.2</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E16" s="1">
+        <x:v>42900</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1225,7 +1393,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId20"/>
+    <x:tablePart r:id="rId21"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1375,14 +1543,33 @@
 </x:worksheet>
 </file>
 
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
 <file path=pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1391,17 +1578,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1410,11 +1600,11 @@
 <file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1423,17 +1613,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1442,11 +1635,11 @@
 <file path=pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1455,17 +1648,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1474,11 +1670,11 @@
 <file path=pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1487,17 +1683,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1506,11 +1705,11 @@
 <file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1519,17 +1718,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1538,11 +1740,11 @@
 <file path=pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1551,17 +1753,20 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1570,11 +1775,11 @@
 <file path=pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:D16"/>
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
-      <x:sharedItems>
+      <x:sharedItems count="5">
         <x:s v="Croissant"/>
         <x:s v="Doughnut"/>
         <x:s v="Bearclaw"/>
@@ -1583,22 +1788,92 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems>
+      <x:sharedItems count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
-        <x:s v="June"/>
+        <x:s v="Jun"/>
       </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
 </file>
 
+<file path=pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15">
+        <x:n v="60.2"/>
+        <x:n v="50.42"/>
+        <x:n v="22.12"/>
+        <x:n v="89.99"/>
+        <x:n v="70"/>
+        <x:n v="75.33"/>
+        <x:n v="10.24"/>
+        <x:n v="33.33"/>
+        <x:n v="25"/>
+        <x:n v="-20.24"/>
+        <x:n v="60"/>
+        <x:n v="24.76"/>
+        <x:n v="0"/>
+        <x:n v="5.19"/>
+        <x:n v="44.2"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
+        <x:d v="2016-04-21T00:00:00"/>
+        <x:d v="2016-05-03T00:00:00"/>
+        <x:d v="2016-06-24T00:00:00"/>
+        <x:d v="2017-04-23T00:00:00"/>
+        <x:d v="2016-05-24T00:00:00"/>
+        <x:d v="2016-06-02T00:00:00"/>
+        <x:d v="2016-04-27T00:00:00"/>
+        <x:d v="2016-05-20T00:00:00"/>
+        <x:d v="2017-06-05T00:00:00"/>
+        <x:d v="2017-04-24T00:00:00"/>
+        <x:d v="2017-05-08T00:00:00"/>
+        <x:d v="2016-06-21T00:00:00"/>
+        <x:d v="2017-04-22T00:00:00"/>
+        <x:d v="2017-05-03T00:00:00"/>
+        <x:d v="2017-06-14T00:00:00"/>
+      </x:sharedItems>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
 <file path=pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1625,4 +1900,8 @@
 
 <file path=pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=pivotCache/pivotCacheRecords8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>

<commit_message>
Fix for example, added test, more complete fix for most options of PT
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -334,7 +334,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -413,7 +413,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" rowHeaderCaption="Pastry name" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -497,7 +497,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -581,7 +581,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
@@ -658,7 +658,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" colHeaderCaption="Measures" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0" colHeaderCaption="Measures">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -734,7 +734,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" fieldListSortAscending="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">

</xml_diff>

<commit_message>
Changed the defaults for the pivot table according to the documentation.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -334,7 +334,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -413,7 +413,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0" rowHeaderCaption="Pastry name">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -497,7 +497,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -581,7 +581,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
@@ -658,7 +658,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0" colHeaderCaption="Measures">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -734,7 +734,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="0">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="5">
     <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">

</xml_diff>

<commit_message>
Fixed some bugs saving pivot table.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -1610,7 +1610,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
@@ -1623,7 +1623,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1645,7 +1645,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
@@ -1658,7 +1658,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1680,7 +1680,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
@@ -1693,7 +1693,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1715,7 +1715,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
@@ -1728,7 +1728,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1750,7 +1750,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
@@ -1763,7 +1763,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1785,7 +1785,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
@@ -1798,7 +1798,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1820,7 +1820,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
@@ -1833,7 +1833,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1855,7 +1855,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="13"/>
     </x:cacheField>
     <x:cacheField name="Quality">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15">
@@ -1884,7 +1884,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
         <x:d v="2016-04-21T00:00:00"/>
         <x:d v="2016-05-03T00:00:00"/>
         <x:d v="2016-06-24T00:00:00"/>

</xml_diff>

<commit_message>
Added tests, XLPivotSortType.Manual renamed to XLPivotSortType.Default
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -15,18 +15,20 @@
     <x:sheet name="pvtFieldAsValueAndLabel" sheetId="8" r:id="rId8"/>
     <x:sheet name="pvtHideSubTotals" sheetId="9" r:id="rId9"/>
     <x:sheet name="pvtFilter" sheetId="10" r:id="rId10"/>
+    <x:sheet name="pvtSort" sheetId="11" r:id="rId11"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId14"/>
-    <x:pivotCache cacheId="1" r:id="rId17"/>
-    <x:pivotCache cacheId="2" r:id="rId20"/>
-    <x:pivotCache cacheId="3" r:id="rId23"/>
-    <x:pivotCache cacheId="4" r:id="rId26"/>
-    <x:pivotCache cacheId="5" r:id="rId29"/>
-    <x:pivotCache cacheId="6" r:id="rId32"/>
-    <x:pivotCache cacheId="7" r:id="rId35"/>
+    <x:pivotCache cacheId="0" r:id="rId15"/>
+    <x:pivotCache cacheId="1" r:id="rId18"/>
+    <x:pivotCache cacheId="2" r:id="rId21"/>
+    <x:pivotCache cacheId="3" r:id="rId24"/>
+    <x:pivotCache cacheId="4" r:id="rId27"/>
+    <x:pivotCache cacheId="5" r:id="rId30"/>
+    <x:pivotCache cacheId="6" r:id="rId33"/>
+    <x:pivotCache cacheId="7" r:id="rId36"/>
+    <x:pivotCache cacheId="8" r:id="rId39"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
@@ -822,6 +824,90 @@
   </x:pageFields>
   <x:dataFields count="1">
     <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+  </x:dataFields>
+  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
+    </x:ext>
+  </x:extLst>
+</x:pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="8" dataCaption="Values" showError="0" missingCaption="" showMissing="1" showItems="0" printDrill="0" showMemberPropertyTips="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" fieldPrintTitles="0" mergeItem="0" indent="0" showEmptyRow="0" showEmptyCol="0" multipleFieldFilters="0" rowHeaderCaption="Pastry name" fieldListSortAscending="0">
+  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:pivotFields count="5">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <x:items count="5">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
+      <x:items count="3">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+  </x:pivotFields>
+  <x:rowFields count="2">
+    <x:field x="0"/>
+    <x:field x="3"/>
+  </x:rowFields>
+  <x:rowItems count="10">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:rowItems>
+  <x:colFields count="1">
+    <x:field x="-2"/>
+  </x:colFields>
+  <x:colItems count="2">
+    <x:i i="0">
+      <x:x v="0"/>
+    </x:i>
+    <x:i i="1">
+      <x:x v="1"/>
+    </x:i>
+  </x:colItems>
+  <x:dataFields count="2">
+    <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -1425,8 +1511,27 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId21"/>
+    <x:tablePart r:id="rId23"/>
   </x:tableParts>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
 </x:worksheet>
 </file>
 
@@ -1906,6 +2011,41 @@
 </x:pivotCacheDefinition>
 </file>
 
+<file path=pivotCache/pivotCacheDefinition9.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:E16"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
 <file path=pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1936,4 +2076,8 @@
 
 <file path=pivotCache/pivotCacheRecords8.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=pivotCache/pivotCacheRecords9.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>

<commit_message>
#598 Fixed some bugs saving pivot table. (#603)
* Fixed some bugs saving pivot table.

* Added test

* Resolve conflict
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -16,27 +16,32 @@
     <x:sheet name="pvtHideSubTotals" sheetId="9" r:id="rId9"/>
     <x:sheet name="pvtFilter" sheetId="10" r:id="rId10"/>
     <x:sheet name="pvtSort" sheetId="11" r:id="rId11"/>
+    <x:sheet name="pvtInteger" sheetId="12" r:id="rId12"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId15"/>
-    <x:pivotCache cacheId="1" r:id="rId18"/>
-    <x:pivotCache cacheId="2" r:id="rId21"/>
-    <x:pivotCache cacheId="3" r:id="rId24"/>
-    <x:pivotCache cacheId="4" r:id="rId27"/>
-    <x:pivotCache cacheId="5" r:id="rId30"/>
-    <x:pivotCache cacheId="6" r:id="rId33"/>
-    <x:pivotCache cacheId="7" r:id="rId36"/>
-    <x:pivotCache cacheId="8" r:id="rId39"/>
+    <x:pivotCache cacheId="0" r:id="rId16"/>
+    <x:pivotCache cacheId="1" r:id="rId19"/>
+    <x:pivotCache cacheId="2" r:id="rId22"/>
+    <x:pivotCache cacheId="3" r:id="rId25"/>
+    <x:pivotCache cacheId="4" r:id="rId28"/>
+    <x:pivotCache cacheId="5" r:id="rId31"/>
+    <x:pivotCache cacheId="6" r:id="rId34"/>
+    <x:pivotCache cacheId="7" r:id="rId37"/>
+    <x:pivotCache cacheId="8" r:id="rId40"/>
+    <x:pivotCache cacheId="9" r:id="rId43"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <x:si>
     <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Code</x:t>
   </x:si>
   <x:si>
     <x:t>NumberOfOrders</x:t>
@@ -146,45 +151,13 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:dxfs count="1">
-    <x:dxf>
-      <x:font>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="11"/>
-        <x:color rgb="FF000000"/>
-        <x:name val="Calibri"/>
-        <x:family val="2"/>
-      </x:font>
-      <x:numFmt numFmtId="14" formatCode="M/d/yyyy"/>
-      <x:fill>
-        <x:patternFill patternType="none"/>
-      </x:fill>
-      <x:border diagonalUp="0" diagonalDown="0">
-        <x:left style="none">
-          <x:color rgb="FF000000"/>
-        </x:left>
-        <x:right style="none">
-          <x:color rgb="FF000000"/>
-        </x:right>
-        <x:top style="none">
-          <x:color rgb="FF000000"/>
-        </x:top>
-        <x:bottom style="none">
-          <x:color rgb="FF000000"/>
-        </x:bottom>
-        <x:diagonal style="none">
-          <x:color rgb="FF000000"/>
-        </x:diagonal>
-      </x:border>
-    </x:dxf>
-  </x:dxfs>
 </x:styleSheet>
 </file>
 
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="5">
+  <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -194,6 +167,7 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Quality" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -229,7 +203,7 @@
     </x:i>
   </x:rowItems>
   <x:colFields count="1">
-    <x:field x="3"/>
+    <x:field x="4"/>
   </x:colFields>
   <x:colItems count="4">
     <x:i>
@@ -246,7 +220,7 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="1">
-    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
+    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="2" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -257,11 +231,20 @@
 </x:pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="9" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="5">
+  <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Code" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -279,13 +262,32 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="15">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+        <x:item x="5"/>
+        <x:item x="6"/>
+        <x:item x="7"/>
+        <x:item x="8"/>
+        <x:item x="9"/>
+        <x:item x="10"/>
+        <x:item x="11"/>
+        <x:item x="12"/>
+        <x:item x="13"/>
+        <x:item x="14"/>
+      </x:items>
+    </x:pivotField>
   </x:pivotFields>
-  <x:rowFields count="2">
+  <x:rowFields count="3">
     <x:field x="0"/>
-    <x:field x="-2"/>
+    <x:field x="1"/>
+    <x:field x="5"/>
   </x:rowFields>
-  <x:rowItems count="6">
+  <x:rowItems count="28">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -304,9 +306,76 @@
     <x:i t="grand">
       <x:x/>
     </x:i>
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
+    <x:i>
+      <x:x v="5"/>
+    </x:i>
+    <x:i>
+      <x:x v="6"/>
+    </x:i>
+    <x:i>
+      <x:x v="7"/>
+    </x:i>
+    <x:i>
+      <x:x v="8"/>
+    </x:i>
+    <x:i>
+      <x:x v="9"/>
+    </x:i>
+    <x:i>
+      <x:x v="10"/>
+    </x:i>
+    <x:i>
+      <x:x v="11"/>
+    </x:i>
+    <x:i>
+      <x:x v="12"/>
+    </x:i>
+    <x:i>
+      <x:x v="13"/>
+    </x:i>
+    <x:i>
+      <x:x v="14"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
   </x:rowItems>
-  <x:colFields count="1">
-    <x:field x="3"/>
+  <x:colFields count="2">
+    <x:field x="4"/>
+    <x:field x="-2"/>
   </x:colFields>
   <x:colItems count="4">
     <x:i>
@@ -323,8 +392,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
-    <x:dataField name="Sum of Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -335,10 +404,10 @@
 </x:pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="5">
+  <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -348,6 +417,86 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+  </x:pivotFields>
+  <x:rowFields count="2">
+    <x:field x="0"/>
+    <x:field x="-2"/>
+  </x:rowFields>
+  <x:rowItems count="6">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:rowItems>
+  <x:colFields count="1">
+    <x:field x="4"/>
+  </x:colFields>
+  <x:colItems count="4">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:colItems>
+  <x:dataFields count="2">
+    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="2" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
+    <x:dataField name="Sum of Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
+  </x:dataFields>
+  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
+    </x:ext>
+  </x:extLst>
+</x:pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:pivotFields count="6">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="5">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -383,7 +532,7 @@
     </x:i>
   </x:rowItems>
   <x:colFields count="2">
-    <x:field x="3"/>
+    <x:field x="4"/>
     <x:field x="-2"/>
   </x:colFields>
   <x:colItems count="4">
@@ -401,9 +550,9 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="3">
-    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
-    <x:dataField name="Sum of Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
-    <x:dataField name="Sum of NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="2" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
+    <x:dataField name="Sum of Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
+    <x:dataField name="Sum of NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -417,7 +566,7 @@
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="5">
+  <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -427,6 +576,7 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -440,7 +590,7 @@
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
-    <x:field x="3"/>
+    <x:field x="4"/>
   </x:rowFields>
   <x:rowItems count="10">
     <x:i>
@@ -486,8 +636,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -501,7 +651,7 @@
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="5">
+  <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item sd="0" x="0"/>
@@ -511,6 +661,7 @@
         <x:item sd="0" x="4"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -524,7 +675,7 @@
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
-    <x:field x="3"/>
+    <x:field x="4"/>
   </x:rowFields>
   <x:rowItems count="10">
     <x:i>
@@ -570,8 +721,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -585,7 +736,7 @@
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="5">
+  <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -595,6 +746,7 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Quality" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -608,7 +760,7 @@
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
-    <x:field x="3"/>
+    <x:field x="4"/>
   </x:rowFields>
   <x:rowItems count="10">
     <x:i>
@@ -662,7 +814,7 @@
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="5">
+  <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -672,6 +824,7 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -688,7 +841,7 @@
   </x:rowFields>
   <x:colFields count="2">
     <x:field x="0"/>
-    <x:field x="3"/>
+    <x:field x="4"/>
   </x:colFields>
   <x:colItems count="10">
     <x:i>
@@ -723,8 +876,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="1" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
-    <x:dataField name="Sum of Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
+    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="2" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
+    <x:dataField name="Sum of Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -738,7 +891,7 @@
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <x:pivotFields count="5">
+  <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item h="1" x="0"/>
@@ -748,9 +901,10 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Quality" axis="axisPage" showAll="0" defaultSubtotal="0">
-      <x:items count="15">
+      <x:items count="16">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
@@ -766,6 +920,7 @@
         <x:item x="12"/>
         <x:item x="13"/>
         <x:item x="14"/>
+        <x:item x="15"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -796,7 +951,7 @@
     </x:pivotField>
   </x:pivotFields>
   <x:rowFields count="1">
-    <x:field x="3"/>
+    <x:field x="4"/>
   </x:rowFields>
   <x:rowItems count="4">
     <x:i>
@@ -819,11 +974,11 @@
   </x:colItems>
   <x:pageFields count="3">
     <x:pageField fld="0" hier="-1"/>
-    <x:pageField fld="2" item="13" hier="-1"/>
-    <x:pageField fld="4" item="13" hier="-1"/>
+    <x:pageField fld="3" item="13" hier="-1"/>
+    <x:pageField fld="5" item="13" hier="-1"/>
   </x:pageFields>
   <x:dataFields count="1">
-    <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -837,7 +992,7 @@
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="8" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="5">
+  <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
@@ -847,6 +1002,7 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
+    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
@@ -860,7 +1016,7 @@
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
-    <x:field x="3"/>
+    <x:field x="4"/>
   </x:rowFields>
   <x:rowItems count="10">
     <x:i>
@@ -906,8 +1062,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="NumberOfOrders" fld="1" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Quality" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -919,14 +1075,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PastrySalesData" displayName="PastrySalesData" ref="A1:E16" totalsRowShown="0">
-  <x:autoFilter ref="A1:E16"/>
-  <x:tableColumns count="5">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PastrySalesData" displayName="PastrySalesData" ref="A1:F17" totalsRowShown="0">
+  <x:autoFilter ref="A1:F17"/>
+  <x:tableColumns count="6">
     <x:tableColumn id="1" name="Name"/>
-    <x:tableColumn id="2" name="NumberOfOrders"/>
-    <x:tableColumn id="3" name="Quality"/>
-    <x:tableColumn id="4" name="Month"/>
-    <x:tableColumn id="5" name="BakeDate" dataDxfId="0"/>
+    <x:tableColumn id="2" name="Code"/>
+    <x:tableColumn id="3" name="NumberOfOrders"/>
+    <x:tableColumn id="4" name="Quality"/>
+    <x:tableColumn id="5" name="Month"/>
+    <x:tableColumn id="6" name="BakeDate"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -1220,20 +1377,21 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E16"/>
+  <x:dimension ref="A1:F17"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.625425" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="19.395425" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.685425" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="10.355425" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="12.735425" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="8.925425" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="19.395425" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="10.685425" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="10.355425" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="12.735425" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -1249,260 +1407,319 @@
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="n">
         <x:v>150</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="n">
+      <x:c r="D2" s="0" t="n">
         <x:v>60.2</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F2" s="1">
+        <x:v>42481</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="E2" s="1">
-        <x:v>42481</x:v>
+      <x:c r="B3" s="0" t="n">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="n">
+        <x:v>50.42</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F3" s="1">
+        <x:v>42493</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:5">
-      <x:c r="A3" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="n">
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="n">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="n">
+        <x:v>22.12</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F4" s="1">
+        <x:v>42545</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="n">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="n">
         <x:v>250</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="n">
-        <x:v>50.42</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
+      <x:c r="D5" s="0" t="n">
+        <x:v>89.99</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="E3" s="1">
-        <x:v>42493</x:v>
+      <x:c r="F5" s="1">
+        <x:v>42848</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="A4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="n">
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="n">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="n">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="n">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F6" s="1">
+        <x:v>42514</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="n">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="n">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="n">
+        <x:v>75.33</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F7" s="1">
+        <x:v>42523</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="n">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="n">
         <x:v>134</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="n">
-        <x:v>22.12</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
+      <x:c r="D8" s="0" t="n">
+        <x:v>10.24</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F8" s="1">
+        <x:v>42487</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="n">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="n">
+        <x:v>184</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="n">
+        <x:v>33.33</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E4" s="1">
-        <x:v>42545</x:v>
+      <x:c r="F9" s="1">
+        <x:v>42510</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="A5" s="0" t="s">
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="n">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="n">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="n">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="n">
-        <x:v>250</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="n">
-        <x:v>89.99</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E5" s="1">
-        <x:v>42848</x:v>
+      <x:c r="F10" s="1">
+        <x:v>42891</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:5">
-      <x:c r="A6" s="0" t="s">
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="n">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="n">
+        <x:v>394</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="n">
+        <x:v>-20.24</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F11" s="1">
+        <x:v>42849</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="n">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="n">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F12" s="1">
+        <x:v>42863</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="n">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="n">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="n">
+        <x:v>24.76</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="n">
-        <x:v>225</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="n">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
+      <x:c r="F13" s="1">
+        <x:v>42542</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="n">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="n">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="E6" s="1">
-        <x:v>42514</x:v>
+      <x:c r="F14" s="1">
+        <x:v>42847</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="A7" s="0" t="s">
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="n">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="n">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="n">
+        <x:v>5.19</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F15" s="1">
+        <x:v>42858</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="n">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="n">
+        <x:v>243</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="n">
+        <x:v>44.2</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="n">
-        <x:v>210</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="n">
-        <x:v>75.33</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E7" s="1">
-        <x:v>42523</x:v>
+      <x:c r="F16" s="1">
+        <x:v>42900</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:5">
-      <x:c r="A8" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="n">
-        <x:v>134</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="n">
-        <x:v>10.24</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E8" s="1">
-        <x:v>42487</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="A9" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="n">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="n">
-        <x:v>33.33</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E9" s="1">
-        <x:v>42510</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5">
-      <x:c r="A10" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="n">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="n">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E10" s="1">
-        <x:v>42891</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="n">
-        <x:v>394</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="n">
-        <x:v>-20.24</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E11" s="1">
-        <x:v>42849</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5">
-      <x:c r="A12" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="n">
-        <x:v>190</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="n">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E12" s="1">
-        <x:v>42863</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5">
-      <x:c r="A13" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="n">
-        <x:v>221</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="n">
-        <x:v>24.76</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E13" s="1">
-        <x:v>42542</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5">
-      <x:c r="A14" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="n">
-        <x:v>135</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E14" s="1">
-        <x:v>42847</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5">
-      <x:c r="A15" s="0" t="s">
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B15" s="0" t="n">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="n">
-        <x:v>5.19</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E15" s="1">
-        <x:v>42858</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:5">
-      <x:c r="A16" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="n">
-        <x:v>243</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="n">
-        <x:v>44.2</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E16" s="1">
-        <x:v>42900</x:v>
+      <x:c r="C17" s="0" t="n">
+        <x:v>255</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="n">
+        <x:v>18.4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1511,12 +1728,31 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId23"/>
+    <x:tablePart r:id="rId26"/>
   </x:tableParts>
 </x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1702,7 +1938,7 @@
 <file path=pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:E16"/>
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -1714,11 +1950,14 @@
         <x:s v="Scone"/>
       </x:sharedItems>
     </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
       <x:sharedItems count="3">
@@ -1728,16 +1967,16 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
 </file>
 
-<file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=pivotCache/pivotCacheDefinition10.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:E16"/>
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -1749,11 +1988,20 @@
         <x:s v="Scone"/>
       </x:sharedItems>
     </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5">
+        <x:n v="101"/>
+        <x:n v="102"/>
+        <x:n v="103"/>
+        <x:n v="104"/>
+        <x:n v="105"/>
+      </x:sharedItems>
+    </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
       <x:sharedItems count="3">
@@ -1763,233 +2011,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:E16"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:E16"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:E16"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:E16"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:E16"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:E16"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15">
-        <x:n v="60.2"/>
-        <x:n v="50.42"/>
-        <x:n v="22.12"/>
-        <x:n v="89.99"/>
-        <x:n v="70"/>
-        <x:n v="75.33"/>
-        <x:n v="10.24"/>
-        <x:n v="33.33"/>
-        <x:n v="25"/>
-        <x:n v="-20.24"/>
-        <x:n v="60"/>
-        <x:n v="24.76"/>
-        <x:n v="0"/>
-        <x:n v="5.19"/>
-        <x:n v="44.2"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
         <x:d v="2016-04-21T00:00:00"/>
         <x:d v="2016-05-03T00:00:00"/>
         <x:d v="2016-06-24T00:00:00"/>
@@ -2011,10 +2033,10 @@
 </x:pivotCacheDefinition>
 </file>
 
-<file path=pivotCache/pivotCacheDefinition9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:E16"/>
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2026,11 +2048,14 @@
         <x:s v="Scone"/>
       </x:sharedItems>
     </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="122" maxValue="394" count="13"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
       <x:sharedItems count="3">
@@ -2040,13 +2065,316 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0" containsNumber="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
 </file>
 
+<file path=pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
+<file path=pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
+<file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
+<file path=pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
+<file path=pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
+<file path=pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16">
+        <x:n v="60.2"/>
+        <x:n v="50.42"/>
+        <x:n v="22.12"/>
+        <x:n v="89.99"/>
+        <x:n v="70"/>
+        <x:n v="75.33"/>
+        <x:n v="10.24"/>
+        <x:n v="33.33"/>
+        <x:n v="25"/>
+        <x:n v="-20.24"/>
+        <x:n v="60"/>
+        <x:n v="24.76"/>
+        <x:n v="0"/>
+        <x:n v="5.19"/>
+        <x:n v="44.2"/>
+        <x:n v="18.4"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
+        <x:d v="2016-04-21T00:00:00"/>
+        <x:d v="2016-05-03T00:00:00"/>
+        <x:d v="2016-06-24T00:00:00"/>
+        <x:d v="2017-04-23T00:00:00"/>
+        <x:d v="2016-05-24T00:00:00"/>
+        <x:d v="2016-06-02T00:00:00"/>
+        <x:d v="2016-04-27T00:00:00"/>
+        <x:d v="2016-05-20T00:00:00"/>
+        <x:d v="2017-06-05T00:00:00"/>
+        <x:d v="2017-04-24T00:00:00"/>
+        <x:d v="2017-05-08T00:00:00"/>
+        <x:d v="2016-06-21T00:00:00"/>
+        <x:d v="2017-04-22T00:00:00"/>
+        <x:d v="2017-05-03T00:00:00"/>
+        <x:d v="2017-06-14T00:00:00"/>
+      </x:sharedItems>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
+<file path=pivotCache/pivotCacheDefinition9.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
 <file path=pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=pivotCache/pivotCacheRecords10.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 

</xml_diff>

<commit_message>
#613 Pivot table Field Settings saving and loading (#616)
* save and load PivotField options

* #613 Pivot table Field Settings saving and loading

* test fixed

* no message
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -158,7 +158,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -167,17 +167,17 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="0"/>
@@ -235,7 +235,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="9" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -244,7 +244,7 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Code" axis="axisRow" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -253,16 +253,16 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="BakeDate" axis="axisRow" defaultSubtotal="0">
       <x:items count="15">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -408,7 +408,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -417,17 +417,17 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -487,7 +487,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -496,17 +496,17 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="0"/>
@@ -567,7 +567,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -576,17 +576,17 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisRow" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -652,7 +652,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" allDrilled="1" defaultSubtotal="0">
       <x:items count="5">
         <x:item sd="0" x="0"/>
         <x:item sd="0" x="1"/>
@@ -661,17 +661,17 @@
         <x:item sd="0" x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisRow" allDrilled="1" defaultSubtotal="0">
       <x:items count="3">
         <x:item sd="0" x="0"/>
         <x:item sd="0" x="1"/>
         <x:item sd="0" x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -737,7 +737,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" dataField="1" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -746,17 +746,17 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisRow" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -815,7 +815,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisCol" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -824,17 +824,17 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="-2"/>
@@ -892,7 +892,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" defaultSubtotal="0">
       <x:items count="5">
         <x:item h="1" x="0"/>
         <x:item x="1"/>
@@ -901,9 +901,9 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" axis="axisPage" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" axis="axisPage" defaultSubtotal="0">
       <x:items count="16">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -923,14 +923,14 @@
         <x:item x="15"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisRow" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" axis="axisPage" showAll="0" defaultSubtotal="0">
+    <x:pivotField name="BakeDate" axis="axisPage" defaultSubtotal="0">
       <x:items count="15">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -993,7 +993,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="8" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" sortType="ascending" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -1002,17 +1002,17 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" showAll="0" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisRow" sortType="descending" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>

</xml_diff>

<commit_message>
Support table sources for pivot tables
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -1938,7 +1938,7 @@
 <file path=pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -1976,7 +1976,7 @@
 <file path=pivotCache/pivotCacheDefinition10.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource name="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2036,7 +2036,7 @@
 <file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2074,7 +2074,7 @@
 <file path=pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2112,7 +2112,7 @@
 <file path=pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2150,7 +2150,7 @@
 <file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2188,7 +2188,7 @@
 <file path=pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2226,7 +2226,7 @@
 <file path=pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2264,7 +2264,7 @@
 <file path=pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2335,7 +2335,7 @@
 <file path=pivotCache/pivotCacheDefinition9.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData!A1:F17"/>
+    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">

</xml_diff>

<commit_message>
Implement pivot table calculated fields.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -392,8 +392,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
+    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -552,7 +552,7 @@
   <x:dataFields count="3">
     <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="2" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
     <x:dataField name="Sum of Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="4"/>
-    <x:dataField name="Sum of NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Sum of NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -636,8 +636,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
+    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -721,8 +721,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
+    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -800,7 +800,7 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="1">
-    <x:dataField name="Name" fld="0" subtotal="count" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Name" fld="0" subtotal="count" showDataAs="normal" baseField="0" baseItem="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -978,7 +978,7 @@
     <x:pageField fld="5" item="13" hier="-1"/>
   </x:pageFields>
   <x:dataFields count="1">
-    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>
@@ -1062,8 +1062,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="NumberOfOrders" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
+    <x:dataField name="Quality" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0"/>
   </x:dataFields>
   <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
   <x:extLst>

</xml_diff>

<commit_message>
Correctly save pivot table row and column field order
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -430,8 +430,8 @@
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="2">
+    <x:field x="-2"/>
     <x:field x="0"/>
-    <x:field x="-2"/>
   </x:rowFields>
   <x:rowItems count="6">
     <x:i>
@@ -840,8 +840,8 @@
     <x:field x="-2"/>
   </x:rowFields>
   <x:colFields count="2">
+    <x:field x="4"/>
     <x:field x="0"/>
-    <x:field x="4"/>
   </x:colFields>
   <x:colItems count="10">
     <x:i>

</xml_diff>

<commit_message>
Set XLPivotField.ShowBlankItems by default to false and fix treatment of defaults from loading file
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -158,7 +158,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -170,7 +170,7 @@
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -235,7 +235,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="9" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -244,7 +244,7 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="Code" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -255,14 +255,14 @@
     </x:pivotField>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="BakeDate" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="15">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -408,7 +408,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -420,7 +420,7 @@
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -487,7 +487,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -499,7 +499,7 @@
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -567,7 +567,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -579,7 +579,7 @@
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -652,7 +652,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" allDrilled="1" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" allDrilled="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item sd="0" x="0"/>
         <x:item sd="0" x="1"/>
@@ -664,7 +664,7 @@
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisRow" allDrilled="1" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisRow" allDrilled="1" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item sd="0" x="0"/>
         <x:item sd="0" x="1"/>
@@ -737,7 +737,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" dataField="1" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -749,7 +749,7 @@
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" defaultSubtotal="0"/>
     <x:pivotField name="Quality" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -815,7 +815,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisCol" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -827,7 +827,7 @@
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -892,7 +892,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
         <x:item h="1" x="0"/>
         <x:item x="1"/>
@@ -903,7 +903,7 @@
     </x:pivotField>
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" axis="axisPage" defaultSubtotal="0">
+    <x:pivotField name="Quality" axis="axisPage" showAll="0" defaultSubtotal="0">
       <x:items count="16">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -923,14 +923,14 @@
         <x:item x="15"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Month" axis="axisRow" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" axis="axisPage" defaultSubtotal="0">
+    <x:pivotField name="BakeDate" axis="axisPage" showAll="0" defaultSubtotal="0">
       <x:items count="15">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -993,7 +993,7 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="8" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" sortType="ascending" defaultSubtotal="0">
+    <x:pivotField name="Name" axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
       <x:items count="5">
         <x:item x="0"/>
         <x:item x="1"/>
@@ -1005,7 +1005,7 @@
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisRow" sortType="descending" defaultSubtotal="0">
+    <x:pivotField name="Month" axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
         <x:item x="1"/>

</xml_diff>

<commit_message>
Fix error by two pivot with one source #1195
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -156,7 +156,7 @@
 
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:location ref="A1:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
@@ -233,7 +233,7 @@
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="9" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:location ref="A1:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
@@ -406,7 +406,7 @@
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:location ref="A1:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
@@ -485,7 +485,7 @@
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:location ref="A1:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
@@ -565,7 +565,7 @@
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:location ref="A1:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="5">
@@ -650,7 +650,7 @@
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:location ref="A1:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" allDrilled="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
@@ -735,7 +735,7 @@
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:location ref="A1:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
@@ -813,7 +813,7 @@
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:location ref="A1:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="5">
@@ -890,7 +890,7 @@
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <x:location ref="A5:K15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
       <x:items count="5">
@@ -991,7 +991,7 @@
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="8" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:location ref="A1:K11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
       <x:items count="5">

</xml_diff>

<commit_message>
Set versioning number to allow enhanced pivot table features
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -1936,7 +1936,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
@@ -1974,7 +1974,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource name="PastrySalesData"/>
   </x:cacheSource>
@@ -2034,7 +2034,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
@@ -2072,7 +2072,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
@@ -2110,7 +2110,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
@@ -2148,7 +2148,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
@@ -2186,7 +2186,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
@@ -2224,7 +2224,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>
@@ -2262,7 +2262,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource name="PastrySalesData"/>
   </x:cacheSource>
@@ -2333,7 +2333,7 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
   </x:cacheSource>

</xml_diff>